<commit_message>
paper and entropy for paper
</commit_message>
<xml_diff>
--- a/dna-methylation/scripts/develop/illumina450k/entropy/plot/scatter_comparison_rows.xlsx
+++ b/dna-methylation/scripts/develop/illumina450k/entropy/plot/scatter_comparison_rows.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\dna-methylation\dna-methylation\scripts\develop\entropy\plot\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Work\dna-methylation\dna-methylation\scripts\develop\illumina450k\entropy\plot\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="16689" yWindow="8863" windowWidth="16226" windowHeight="9051"/>
+    <workbookView xWindow="16695" yWindow="8865" windowWidth="16230" windowHeight="9045"/>
   </bookViews>
   <sheets>
     <sheet name="i" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
   <si>
     <t>begins</t>
   </si>
@@ -34,6 +34,12 @@
   </si>
   <si>
     <t>entropy</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>reverses</t>
   </si>
 </sst>
 </file>
@@ -65,7 +71,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -88,13 +94,27 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -401,15 +421,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M11" sqref="M11"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="20.53515625" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="20.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -419,8 +439,11 @@
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="D1" s="2" t="s">
+        <v>6</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -429,6 +452,9 @@
       </c>
       <c r="C2" t="s">
         <v>3</v>
+      </c>
+      <c r="D2" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>